<commit_message>
fixed formulas on Km
</commit_message>
<xml_diff>
--- a/Convert Km to Yards to Chains.xlsx
+++ b/Convert Km to Yards to Chains.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://networkrail-my.sharepoint.com/personal/swainwr6_networkrail_co_uk/Documents/H Files/Power BI Projects/Projects/Milage Converter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="856" documentId="8_{BC24BA6F-3815-4438-A7F3-2B89B837400B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75D8FF2C-9E63-41BF-B2C1-503F10EAE249}"/>
+  <xr:revisionPtr revIDLastSave="940" documentId="8_{BC24BA6F-3815-4438-A7F3-2B89B837400B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CC12B0D-5E0D-4D23-AF0B-2DF162A77897}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8384C43C-9482-4A36-9CEA-B68BE1CE09A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Converter" sheetId="3" r:id="rId1"/>
-    <sheet name="Lookups" sheetId="4" r:id="rId2"/>
-    <sheet name="Backend Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Converter" sheetId="5" r:id="rId1"/>
+    <sheet name="Backend Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Enter Kilometers here</t>
   </si>
@@ -60,9 +59,6 @@
   </si>
   <si>
     <t>Kilometers</t>
-  </si>
-  <si>
-    <t>RedAmder Gren</t>
   </si>
   <si>
     <t>Locs</t>
@@ -231,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -254,12 +250,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,12 +326,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -321,14 +361,32 @@
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -649,53 +707,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E27471-C394-4F20-A53F-63319503FDE9}">
-  <dimension ref="B1:L28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB53802-04C8-4B6E-AAE5-1F76EBF12F7C}">
+  <dimension ref="B1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="15" customWidth="1"/>
-    <col min="2" max="4" width="20.5703125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" style="15" customWidth="1"/>
-    <col min="6" max="8" width="20.5703125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" style="15" customWidth="1"/>
-    <col min="10" max="12" width="20.5703125" style="15" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="3.140625" style="13" customWidth="1"/>
+    <col min="2" max="4" width="20.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" style="13" customWidth="1"/>
+    <col min="6" max="8" width="20.5703125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" style="13" customWidth="1"/>
+    <col min="10" max="12" width="20.5703125" style="13" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="13"/>
+    <col min="16" max="16" width="13.5703125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="13" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="1" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="F2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="J2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="2:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -704,7 +765,7 @@
       <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -713,860 +774,872 @@
       <c r="L3" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13">
-        <v>10</v>
-      </c>
-      <c r="C4" s="20">
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+    </row>
+    <row r="4" spans="2:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>10</v>
+      </c>
+      <c r="C4" s="18">
         <f>CONVERT(B4,"km","mi")</f>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D4" s="14" t="str">
-        <f>CONCATENATE(INT((B4)*1000/0.9144/1760),"m ",ROUND(80*(((B4)*1000/0.9144/1760)-INT((B4)*1000/0.9144/1760)),0),"ch")</f>
-        <v>6m 17ch</v>
-      </c>
-      <c r="F4" s="13">
-        <v>10</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="D4" s="12" t="str">
+        <f>CONCATENATE(INT((B4)*1000/0.9144/1760),".",ROUND(80*(((B4)*1000/0.9144/1760)-INT((B4)*1000/0.9144/1760)),0))</f>
+        <v>6.17</v>
+      </c>
+      <c r="F4" s="11">
+        <v>10</v>
+      </c>
+      <c r="G4" s="18">
         <f>CONVERT(H4,"km","mi")</f>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H4" s="14">
-        <f>CONCATENATE(INT((F4)/1000*0.9144*1760),ROUND(80/(((F4)/1000*0.9144*1760)-INT((F4)/1000*0.9144*1760)),0))/100</f>
-        <v>168.56</v>
-      </c>
-      <c r="J4" s="16">
-        <v>10</v>
-      </c>
-      <c r="K4" s="20" t="str">
-        <f>INT(SUM(J4/1000/1.093*1770))&amp;"."&amp;TEXT(MOD(SUM(J4/1000/1.093),1770),"00")</f>
-        <v>16.00</v>
-      </c>
-      <c r="L4" s="14" t="str">
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H4" s="12" t="str">
+        <f>CONCATENATE(INT((F4)/1000*0.9144*1760),".",ROUND(80/(((F4)/1000*0.9144*1760)-INT((F4)/1000*0.9144*1760)),0))</f>
+        <v>16.856</v>
+      </c>
+      <c r="J4" s="14">
+        <v>10</v>
+      </c>
+      <c r="K4" s="12">
+        <f>CONVERT(J4,"mi","km")</f>
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L4" s="12" t="str">
         <f>CONCATENATE(INT((K4)*1000/0.9144/1760),"m ",ROUND(80*(((K4)*1000/0.9144/1760)-INT((K4)*1000/0.9144/1760)),0),"ch")</f>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="13">
-        <v>10</v>
-      </c>
-      <c r="C7" s="20">
+        <v>10m 0ch</v>
+      </c>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+    </row>
+    <row r="5" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="27"/>
+    </row>
+    <row r="6" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18">
         <f t="shared" ref="C7:C28" si="0">CONVERT(B7,"km","mi")</f>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D7" s="14" t="str">
-        <f t="shared" ref="D7:D28" si="1">CONCATENATE(INT((B7)*1000/0.9144/1760),"m ",ROUND(80*(((B7)*1000/0.9144/1760)-INT((B7)*1000/0.9144/1760)),0),"ch")</f>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="13">
-        <v>10</v>
-      </c>
-      <c r="G7" s="20">
+      <c r="D7" s="12" t="str">
+        <f t="shared" ref="D7:D28" si="1">CONCATENATE(INT((B7)*1000/0.9144/1760),".",ROUND(80*(((B7)*1000/0.9144/1760)-INT((B7)*1000/0.9144/1760)),0))</f>
+        <v>6.17</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="11">
+        <v>10</v>
+      </c>
+      <c r="G7" s="18">
         <f t="shared" ref="G7:G28" si="2">CONVERT(H7,"km","mi")</f>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H7" s="14">
-        <f t="shared" ref="H7:H28" si="3">CONCATENATE(INT((F7)/1000*0.9144*1760),ROUND(80/(((F7)/1000*0.9144*1760)-INT((F7)/1000*0.9144*1760)),0))/100</f>
-        <v>168.56</v>
-      </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16">
-        <v>10</v>
-      </c>
-      <c r="K7" s="20" t="str">
-        <f t="shared" ref="K7:K28" si="4">INT(SUM(J7/1000/1.093*1770))&amp;"."&amp;TEXT(MOD(SUM(J7/1000/1.093),1770),"00")</f>
-        <v>16.00</v>
-      </c>
-      <c r="L7" s="14" t="str">
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H7" s="12" t="str">
+        <f t="shared" ref="H7:H28" si="3">CONCATENATE(INT((F7)/1000*0.9144*1760),".",ROUND(80/(((F7)/1000*0.9144*1760)-INT((F7)/1000*0.9144*1760)),0))</f>
+        <v>16.856</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14">
+        <v>10</v>
+      </c>
+      <c r="K7" s="18">
+        <f t="shared" ref="K7:K28" si="4">CONVERT(J7,"mi","km")</f>
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L7" s="12" t="str">
         <f t="shared" ref="L7:L28" si="5">CONCATENATE(INT((K7)*1000/0.9144/1760),"m ",ROUND(80*(((K7)*1000/0.9144/1760)-INT((K7)*1000/0.9144/1760)),0),"ch")</f>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="13">
-        <v>10</v>
-      </c>
-      <c r="C8" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D8" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="13">
-        <v>10</v>
-      </c>
-      <c r="G8" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H8" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16">
-        <v>10</v>
-      </c>
-      <c r="K8" s="20" t="str">
+      <c r="D8" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="11">
+        <v>10</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14">
+        <v>10</v>
+      </c>
+      <c r="K8" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L8" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L8" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="13">
-        <v>10</v>
-      </c>
-      <c r="C9" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D9" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="13">
-        <v>10</v>
-      </c>
-      <c r="G9" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H9" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16">
-        <v>10</v>
-      </c>
-      <c r="K9" s="20" t="str">
+      <c r="D9" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="11">
+        <v>10</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H9" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14">
+        <v>10</v>
+      </c>
+      <c r="K9" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L9" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L9" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="13">
-        <v>10</v>
-      </c>
-      <c r="C10" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D10" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="13">
-        <v>10</v>
-      </c>
-      <c r="G10" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H10" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16">
-        <v>10</v>
-      </c>
-      <c r="K10" s="20" t="str">
+      <c r="D10" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="11">
+        <v>10</v>
+      </c>
+      <c r="G10" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H10" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14">
+        <v>10</v>
+      </c>
+      <c r="K10" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L10" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L10" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
-        <v>10</v>
-      </c>
-      <c r="C11" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D11" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="13">
-        <v>10</v>
-      </c>
-      <c r="G11" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H11" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="16">
-        <v>10</v>
-      </c>
-      <c r="K11" s="20" t="str">
+      <c r="D11" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H11" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14">
+        <v>10</v>
+      </c>
+      <c r="K11" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L11" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L11" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="13">
-        <v>10</v>
-      </c>
-      <c r="C12" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D12" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="13">
-        <v>10</v>
-      </c>
-      <c r="G12" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="16">
-        <v>10</v>
-      </c>
-      <c r="K12" s="20" t="str">
+      <c r="D12" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11">
+        <v>10</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H12" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14">
+        <v>10</v>
+      </c>
+      <c r="K12" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L12" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L12" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
-        <v>10</v>
-      </c>
-      <c r="C13" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D13" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="13">
-        <v>10</v>
-      </c>
-      <c r="G13" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H13" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16">
-        <v>10</v>
-      </c>
-      <c r="K13" s="20" t="str">
+      <c r="D13" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="11">
+        <v>10</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H13" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14">
+        <v>10</v>
+      </c>
+      <c r="K13" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L13" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L13" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="13">
-        <v>10</v>
-      </c>
-      <c r="C14" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11">
+        <v>10</v>
+      </c>
+      <c r="C14" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D14" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="13">
-        <v>10</v>
-      </c>
-      <c r="G14" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H14" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16">
-        <v>10</v>
-      </c>
-      <c r="K14" s="20" t="str">
+      <c r="D14" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11">
+        <v>10</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H14" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14">
+        <v>10</v>
+      </c>
+      <c r="K14" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L14" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L14" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
-        <v>10</v>
-      </c>
-      <c r="C15" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11">
+        <v>10</v>
+      </c>
+      <c r="C15" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D15" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="13">
-        <v>10</v>
-      </c>
-      <c r="G15" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H15" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16">
-        <v>10</v>
-      </c>
-      <c r="K15" s="20" t="str">
+      <c r="D15" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="11">
+        <v>10</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H15" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14">
+        <v>10</v>
+      </c>
+      <c r="K15" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L15" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L15" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="13">
-        <v>10</v>
-      </c>
-      <c r="C16" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <v>10</v>
+      </c>
+      <c r="C16" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D16" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="13">
-        <v>10</v>
-      </c>
-      <c r="G16" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H16" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="16">
-        <v>10</v>
-      </c>
-      <c r="K16" s="20" t="str">
+      <c r="D16" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="11">
+        <v>10</v>
+      </c>
+      <c r="G16" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H16" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14">
+        <v>10</v>
+      </c>
+      <c r="K16" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L16" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L16" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="13">
-        <v>10</v>
-      </c>
-      <c r="C17" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <v>10</v>
+      </c>
+      <c r="C17" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D17" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="13">
-        <v>10</v>
-      </c>
-      <c r="G17" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H17" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16">
-        <v>10</v>
-      </c>
-      <c r="K17" s="20" t="str">
+      <c r="D17" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="11">
+        <v>10</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H17" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14">
+        <v>10</v>
+      </c>
+      <c r="K17" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L17" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L17" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="13">
-        <v>10</v>
-      </c>
-      <c r="C18" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <v>10</v>
+      </c>
+      <c r="C18" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D18" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="13">
-        <v>10</v>
-      </c>
-      <c r="G18" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H18" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16">
-        <v>10</v>
-      </c>
-      <c r="K18" s="20" t="str">
+      <c r="D18" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="11">
+        <v>10</v>
+      </c>
+      <c r="G18" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H18" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14">
+        <v>10</v>
+      </c>
+      <c r="K18" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L18" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L18" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="13">
-        <v>10</v>
-      </c>
-      <c r="C19" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <v>10</v>
+      </c>
+      <c r="C19" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D19" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="13">
-        <v>10</v>
-      </c>
-      <c r="G19" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H19" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16">
-        <v>10</v>
-      </c>
-      <c r="K19" s="20" t="str">
+      <c r="D19" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="11">
+        <v>10</v>
+      </c>
+      <c r="G19" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H19" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14">
+        <v>10</v>
+      </c>
+      <c r="K19" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L19" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L19" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="13">
-        <v>10</v>
-      </c>
-      <c r="C20" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <v>10</v>
+      </c>
+      <c r="C20" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D20" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="13">
-        <v>10</v>
-      </c>
-      <c r="G20" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H20" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16">
-        <v>10</v>
-      </c>
-      <c r="K20" s="20" t="str">
+      <c r="D20" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="11">
+        <v>10</v>
+      </c>
+      <c r="G20" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H20" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14">
+        <v>10</v>
+      </c>
+      <c r="K20" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L20" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L20" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="13">
-        <v>10</v>
-      </c>
-      <c r="C21" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <v>10</v>
+      </c>
+      <c r="C21" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D21" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="13">
-        <v>10</v>
-      </c>
-      <c r="G21" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H21" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="16">
-        <v>10</v>
-      </c>
-      <c r="K21" s="20" t="str">
+      <c r="D21" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="11">
+        <v>10</v>
+      </c>
+      <c r="G21" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H21" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14">
+        <v>10</v>
+      </c>
+      <c r="K21" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L21" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L21" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="13">
-        <v>10</v>
-      </c>
-      <c r="C22" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
+        <v>10</v>
+      </c>
+      <c r="C22" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D22" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="13">
-        <v>10</v>
-      </c>
-      <c r="G22" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H22" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16">
-        <v>10</v>
-      </c>
-      <c r="K22" s="20" t="str">
+      <c r="D22" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="11">
+        <v>10</v>
+      </c>
+      <c r="G22" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H22" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14">
+        <v>10</v>
+      </c>
+      <c r="K22" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L22" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L22" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
-        <v>10</v>
-      </c>
-      <c r="C23" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>10</v>
+      </c>
+      <c r="C23" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D23" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E23" s="15"/>
-      <c r="F23" s="13">
-        <v>10</v>
-      </c>
-      <c r="G23" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H23" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I23" s="15"/>
-      <c r="J23" s="16">
-        <v>10</v>
-      </c>
-      <c r="K23" s="20" t="str">
+      <c r="D23" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="11">
+        <v>10</v>
+      </c>
+      <c r="G23" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H23" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I23" s="13"/>
+      <c r="J23" s="14">
+        <v>10</v>
+      </c>
+      <c r="K23" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L23" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L23" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
-        <v>10</v>
-      </c>
-      <c r="C24" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <v>10</v>
+      </c>
+      <c r="C24" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D24" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E24" s="15"/>
-      <c r="F24" s="13">
-        <v>10</v>
-      </c>
-      <c r="G24" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H24" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="16">
-        <v>10</v>
-      </c>
-      <c r="K24" s="20" t="str">
+      <c r="D24" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="11">
+        <v>10</v>
+      </c>
+      <c r="G24" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H24" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I24" s="13"/>
+      <c r="J24" s="14">
+        <v>10</v>
+      </c>
+      <c r="K24" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L24" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L24" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="13">
-        <v>10</v>
-      </c>
-      <c r="C25" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>10</v>
+      </c>
+      <c r="C25" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D25" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="13">
-        <v>10</v>
-      </c>
-      <c r="G25" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H25" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16">
-        <v>10</v>
-      </c>
-      <c r="K25" s="20" t="str">
+      <c r="D25" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="11">
+        <v>10</v>
+      </c>
+      <c r="G25" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H25" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14">
+        <v>10</v>
+      </c>
+      <c r="K25" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L25" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L25" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="13">
-        <v>10</v>
-      </c>
-      <c r="C26" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>10</v>
+      </c>
+      <c r="C26" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D26" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="13">
-        <v>10</v>
-      </c>
-      <c r="G26" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H26" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="16">
-        <v>10</v>
-      </c>
-      <c r="K26" s="20" t="str">
+      <c r="D26" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="11">
+        <v>10</v>
+      </c>
+      <c r="G26" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H26" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14">
+        <v>10</v>
+      </c>
+      <c r="K26" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L26" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L26" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="13">
-        <v>10</v>
-      </c>
-      <c r="C27" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <v>10</v>
+      </c>
+      <c r="C27" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D27" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="13">
-        <v>10</v>
-      </c>
-      <c r="G27" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H27" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="16">
-        <v>10</v>
-      </c>
-      <c r="K27" s="20" t="str">
+      <c r="D27" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="11">
+        <v>10</v>
+      </c>
+      <c r="G27" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H27" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14">
+        <v>10</v>
+      </c>
+      <c r="K27" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L27" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L27" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="13">
-        <v>10</v>
-      </c>
-      <c r="C28" s="20">
+        <v>10m 0ch</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <v>10</v>
+      </c>
+      <c r="C28" s="18">
         <f t="shared" si="0"/>
         <v>6.2137119223733395</v>
       </c>
-      <c r="D28" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v>6m 17ch</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="13">
-        <v>10</v>
-      </c>
-      <c r="G28" s="20">
-        <f t="shared" si="2"/>
-        <v>104.73832816352501</v>
-      </c>
-      <c r="H28" s="14">
-        <f t="shared" si="3"/>
-        <v>168.56</v>
-      </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="16">
-        <v>10</v>
-      </c>
-      <c r="K28" s="20" t="str">
+      <c r="D28" s="12" t="str">
+        <f t="shared" si="1"/>
+        <v>6.17</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="11">
+        <v>10</v>
+      </c>
+      <c r="G28" s="18">
+        <f t="shared" si="2"/>
+        <v>10.473832816352504</v>
+      </c>
+      <c r="H28" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v>16.856</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14">
+        <v>10</v>
+      </c>
+      <c r="K28" s="18">
         <f t="shared" si="4"/>
-        <v>16.00</v>
-      </c>
-      <c r="L28" s="14" t="str">
+        <v>16.093440000000001</v>
+      </c>
+      <c r="L28" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>9m 75ch</v>
+        <v>10m 0ch</v>
       </c>
     </row>
   </sheetData>
@@ -1579,26 +1652,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EB958C-6F0D-40B0-8E4F-C64ABC16D7FB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC9A328-37AD-4A75-9E1E-6279DEC27379}">
   <dimension ref="A1:L103"/>
   <sheetViews>
@@ -1617,37 +1670,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="G2">
         <v>1</v>
       </c>
@@ -1662,22 +1715,22 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1691,7 +1744,7 @@
         <v>3520</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1722,7 +1775,7 @@
         <v>7040</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1753,7 +1806,7 @@
         <v>14080</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1812,7 +1865,7 @@
         <v>56320</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1843,7 +1896,7 @@
         <v>112640</v>
       </c>
       <c r="L8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3358,18 +3411,18 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="10">
+      <c r="A83" s="8">
         <v>80</v>
       </c>
-      <c r="B83" s="10">
+      <c r="B83" s="8">
         <f t="shared" ref="B83" si="6">A83*22</f>
         <v>1760</v>
       </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="10">
+      <c r="D83" s="8">
         <v>80</v>
       </c>
-      <c r="E83" s="11">
+      <c r="E83" s="9">
         <f t="shared" ref="E83:E103" si="7">D83/0.03</f>
         <v>2666.666666666667</v>
       </c>
@@ -3628,12 +3681,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="af32717b-85d4-46b0-82d8-410bc3119485" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52a0e33b-8272-48f8-bd27-682bbb4d8ddd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3885,20 +3940,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="af32717b-85d4-46b0-82d8-410bc3119485" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52a0e33b-8272-48f8-bd27-682bbb4d8ddd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B63EEFF-B1FB-420F-9960-E8555A106148}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE097FB-FD39-4C3F-A857-C1EAB028DD45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="af32717b-85d4-46b0-82d8-410bc3119485"/>
+    <ds:schemaRef ds:uri="52a0e33b-8272-48f8-bd27-682bbb4d8ddd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3924,12 +3980,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE097FB-FD39-4C3F-A857-C1EAB028DD45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B63EEFF-B1FB-420F-9960-E8555A106148}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="af32717b-85d4-46b0-82d8-410bc3119485"/>
-    <ds:schemaRef ds:uri="52a0e33b-8272-48f8-bd27-682bbb4d8ddd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Convert Km to Yards to Chains
Convert Km to Yards to Chains
</commit_message>
<xml_diff>
--- a/Convert Km to Yards to Chains.xlsx
+++ b/Convert Km to Yards to Chains.xlsx
@@ -364,12 +364,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,6 +381,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -730,30 +730,30 @@
   <sheetData>
     <row r="1" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
-      <c r="F2" s="24" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+      <c r="F2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="J2" s="24" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="J2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="2:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="16" t="s">
@@ -821,7 +821,7 @@
       <c r="R4" s="15"/>
     </row>
     <row r="5" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H5" s="27"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="2:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
@@ -1670,13 +1670,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="G1" t="s">
         <v>9</v>
       </c>
@@ -1694,10 +1694,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -3681,14 +3681,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="af32717b-85d4-46b0-82d8-410bc3119485" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52a0e33b-8272-48f8-bd27-682bbb4d8ddd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3940,21 +3938,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="af32717b-85d4-46b0-82d8-410bc3119485" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="52a0e33b-8272-48f8-bd27-682bbb4d8ddd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE097FB-FD39-4C3F-A857-C1EAB028DD45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B63EEFF-B1FB-420F-9960-E8555A106148}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="af32717b-85d4-46b0-82d8-410bc3119485"/>
-    <ds:schemaRef ds:uri="52a0e33b-8272-48f8-bd27-682bbb4d8ddd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3980,9 +3977,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B63EEFF-B1FB-420F-9960-E8555A106148}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BE097FB-FD39-4C3F-A857-C1EAB028DD45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="af32717b-85d4-46b0-82d8-410bc3119485"/>
+    <ds:schemaRef ds:uri="52a0e33b-8272-48f8-bd27-682bbb4d8ddd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>